<commit_message>
data: add time data for serial python and parallel pyomp implementations for pi computation
</commit_message>
<xml_diff>
--- a/Experiments/OpenMP_Comparisons.xlsx
+++ b/Experiments/OpenMP_Comparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhish17\Desktop\PL\Project\Parallel-Programming-Constructs\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F411287-1AC3-40C8-AB18-39EF00BDB4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12566DF-941E-4F57-9E34-FEF608E42FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>Program</t>
   </si>
@@ -49,9 +49,6 @@
     <t>PyOMP</t>
   </si>
   <si>
-    <t>PyOMP with JIT</t>
-  </si>
-  <si>
     <t>Matrix Multiplication</t>
   </si>
   <si>
@@ -113,6 +110,15 @@
   </si>
   <si>
     <t>C++ Parallel (16 threads)</t>
+  </si>
+  <si>
+    <t>PyOMP (16 threads)</t>
+  </si>
+  <si>
+    <t>The PyOMP time values are without the JIT compilation time</t>
+  </si>
+  <si>
+    <t>Python (Serial)</t>
   </si>
 </sst>
 </file>
@@ -445,86 +451,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4316CE6-39B2-44DD-8FD3-04F419982031}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
     <col min="2" max="2" width="50.5546875" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -535,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,70 +556,73 @@
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
     <col min="2" max="2" width="20.21875" customWidth="1"/>
     <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2.173667</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>5.9428669999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>6.1567999999999998E-2</v>
       </c>
+      <c r="D3">
+        <v>1.6643667000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.41336499999999998</v>
+      </c>
       <c r="F3">
-        <v>0.41336499999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.8699724360000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>1.3365E-2</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>4.3808E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>8.2858199999999993</v>
@@ -617,13 +630,13 @@
       <c r="C5">
         <v>2.7793749999999999</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>15.374567000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>5.2700769999999997</v>
@@ -631,18 +644,18 @@
       <c r="C6">
         <v>2.0762990000000001</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>7.9477019999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>2.6113999999999998E-2</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>0.106588</v>
       </c>
     </row>
@@ -653,146 +666,244 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625CEBF0-B641-439B-B080-CB4876D8D045}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0.41121000000000002</v>
       </c>
       <c r="B2">
         <v>5.7464000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>1.9570112228393499E-2</v>
+      </c>
+      <c r="D2">
+        <v>5.8453071117401096</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.42094300000000001</v>
       </c>
       <c r="B3">
         <v>6.0519000000000003E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1.4625072479248E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.8402287960052401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.41970600000000002</v>
       </c>
       <c r="B4">
         <v>6.7448999999999995E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>2.4492025375366201E-2</v>
+      </c>
+      <c r="D4">
+        <v>5.8900222778320304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.42357</v>
       </c>
       <c r="B5">
         <v>5.5787999999999997E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1.46269798278808E-2</v>
+      </c>
+      <c r="D5">
+        <v>5.8570322990417401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.41464400000000001</v>
       </c>
       <c r="B6">
         <v>7.9546000000000006E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1.6587018966674801E-2</v>
+      </c>
+      <c r="D6">
+        <v>5.7842073440551696</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.41665400000000002</v>
       </c>
       <c r="B7">
         <v>6.1622999999999997E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1.44770145416259E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.8378751277923504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0.412854</v>
       </c>
       <c r="B8">
         <v>6.2451E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>1.5317916870117101E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.8321020603179896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0.41177200000000003</v>
       </c>
       <c r="B9">
         <v>6.2102999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1.6975879669189401E-2</v>
+      </c>
+      <c r="D9">
+        <v>6.0616035461425701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0.41416900000000001</v>
       </c>
       <c r="B10">
         <v>5.2070999999999999E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>1.7638921737670898E-2</v>
+      </c>
+      <c r="D10">
+        <v>5.7991998195648096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0.41565400000000002</v>
       </c>
       <c r="B11">
         <v>6.3840999999999995E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>1.6988039016723602E-2</v>
+      </c>
+      <c r="D11">
+        <v>5.8336338996887198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.420653</v>
       </c>
       <c r="B12">
         <v>5.9910999999999999E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>1.5735864639282199E-2</v>
+      </c>
+      <c r="D12">
+        <v>5.8899166584014804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0.38577400000000001</v>
       </c>
       <c r="B13">
         <v>6.7740999999999996E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1.6485929489135701E-2</v>
+      </c>
+      <c r="D13">
+        <v>5.80106353759765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0.42255500000000001</v>
       </c>
       <c r="B14">
         <v>6.1046999999999997E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>1.5494108200073201E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.8232157230377197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.42057499999999998</v>
       </c>
       <c r="B15">
         <v>5.5365999999999999E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>1.54900550842285E-2</v>
+      </c>
+      <c r="D15">
+        <v>5.9568130970001203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0.38974500000000001</v>
       </c>
       <c r="B16">
         <v>5.6604000000000002E-2</v>
+      </c>
+      <c r="C16">
+        <v>1.5150070190429601E-2</v>
+      </c>
+      <c r="D16">
+        <v>5.9973652362823398</v>
       </c>
     </row>
   </sheetData>
@@ -816,10 +927,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -963,10 +1074,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1110,10 +1221,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1260,13 +1371,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1458,13 +1569,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
data: add result images for comparisons
</commit_message>
<xml_diff>
--- a/Experiments/OpenMP_Comparisons.xlsx
+++ b/Experiments/OpenMP_Comparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidhish17\Desktop\PL\Project\Parallel-Programming-Constructs\Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12566DF-941E-4F57-9E34-FEF608E42FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A895505-E802-439B-BF1C-55A8550D7757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="8" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625CEBF0-B641-439B-B080-CB4876D8D045}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>